<commit_message>
Make the fake CO2RR look better
</commit_message>
<xml_diff>
--- a/volcanos_parsed.xlsx
+++ b/volcanos_parsed.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KTran/Google_Drive/Misc_Docs/Volcanos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KTran/Google_Drive/Misc_Docs/Literature_Figures/volcanos/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="440" windowWidth="17060" windowHeight="15480" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28260" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OER" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="131">
   <si>
     <t>CoOx-(a)</t>
   </si>
@@ -465,6 +465,9 @@
   </si>
   <si>
     <t>Zenith</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -878,11 +881,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1561834016"/>
-        <c:axId val="1562024640"/>
+        <c:axId val="1535015328"/>
+        <c:axId val="1449081376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1561834016"/>
+        <c:axId val="1535015328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.4"/>
@@ -927,7 +930,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -993,13 +995,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1562024640"/>
+        <c:crossAx val="1449081376"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.4"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1562024640"/>
+        <c:axId val="1449081376"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="0.85"/>
@@ -1033,7 +1035,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1100,7 +1101,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1561834016"/>
+        <c:crossAx val="1535015328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1395,11 +1396,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1532559440"/>
-        <c:axId val="1532562832"/>
+        <c:axId val="1534981664"/>
+        <c:axId val="1485570176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1532559440"/>
+        <c:axId val="1534981664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1438,7 +1439,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1504,12 +1504,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1532562832"/>
+        <c:crossAx val="1485570176"/>
         <c:crossesAt val="-2.5"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1532562832"/>
+        <c:axId val="1485570176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,7 +1615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1532559440"/>
+        <c:crossAx val="1534981664"/>
         <c:crossesAt val="-4.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2048,11 +2048,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1532694176"/>
-        <c:axId val="1532697568"/>
+        <c:axId val="1564948384"/>
+        <c:axId val="1564776112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1532694176"/>
+        <c:axId val="1564948384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.8"/>
@@ -2093,7 +2093,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2159,13 +2158,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1532697568"/>
+        <c:crossAx val="1564776112"/>
         <c:crossesAt val="1.0E-8"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.4"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1532697568"/>
+        <c:axId val="1564776112"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2273,7 +2272,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1532694176"/>
+        <c:crossAx val="1564948384"/>
         <c:crossesAt val="-1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2520,28 +2519,28 @@
                 <c:pt idx="1">
                   <c:v>8.75680941901776E-8</c:v>
                 </c:pt>
-                <c:pt idx="2" formatCode="General">
+                <c:pt idx="2">
                   <c:v>1.29118365092215E-6</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="General">
+                <c:pt idx="3">
                   <c:v>4.89370742451432E-6</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="General">
+                <c:pt idx="4">
                   <c:v>6.94105472727538E-6</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="General">
+                <c:pt idx="5">
                   <c:v>0.00139246766815199</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="General">
+                <c:pt idx="6">
                   <c:v>0.00103559232881604</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="General">
+                <c:pt idx="7">
                   <c:v>0.00245126924770454</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="8">
                   <c:v>0.000781250803324243</c:v>
                 </c:pt>
-                <c:pt idx="9" formatCode="General">
+                <c:pt idx="9">
                   <c:v>0.00048135923527038</c:v>
                 </c:pt>
               </c:numCache>
@@ -2664,7 +2663,7 @@
             <c:numRef>
               <c:f>CO2RR!$B$11:$B$19</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.00048135923527038</c:v>
@@ -2684,13 +2683,13 @@
                 <c:pt idx="5">
                   <c:v>2.04721308556154E-6</c:v>
                 </c:pt>
-                <c:pt idx="6" formatCode="0.00E+00">
+                <c:pt idx="6">
                   <c:v>2.58343974842545E-7</c:v>
                 </c:pt>
-                <c:pt idx="7" formatCode="0.00E+00">
+                <c:pt idx="7">
                   <c:v>1.61329941902728E-7</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="0.00E+00">
+                <c:pt idx="8">
                   <c:v>1.41475218609214E-8</c:v>
                 </c:pt>
               </c:numCache>
@@ -2706,11 +2705,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1564361184"/>
-        <c:axId val="1564364944"/>
+        <c:axId val="1528090080"/>
+        <c:axId val="1527858576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1564361184"/>
+        <c:axId val="1528090080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -2817,13 +2816,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1564364944"/>
+        <c:crossAx val="1527858576"/>
         <c:crossesAt val="1.0E-8"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.4"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1564364944"/>
+        <c:axId val="1527858576"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2931,7 +2930,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1564361184"/>
+        <c:crossAx val="1528090080"/>
         <c:crossesAt val="-1.5"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7476,7 +7475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -7574,10 +7573,11 @@
         <f>LN(B2)</f>
         <v>-15.553346942875836</v>
       </c>
-      <c r="O2" s="11">
+      <c r="O2" s="10">
         <f t="shared" ref="O2:O12" si="0">EXP(G$2*C2+H$2)</f>
         <v>1.3758404735445592E-8</v>
       </c>
+      <c r="P2" s="10"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -7619,16 +7619,17 @@
         <f t="shared" ref="N3:N19" si="1">LN(B3)</f>
         <v>-16.250849126922169</v>
       </c>
-      <c r="O3" s="11">
+      <c r="O3" s="10">
         <f t="shared" si="0"/>
         <v>1.8331631102289673E-6</v>
       </c>
+      <c r="P3" s="10"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="13">
         <v>1.29118365092215E-6</v>
       </c>
       <c r="C4">
@@ -7664,16 +7665,17 @@
         <f t="shared" si="1"/>
         <v>-13.559951201436114</v>
       </c>
-      <c r="O4" s="11">
+      <c r="O4" s="10">
         <f t="shared" si="0"/>
         <v>5.305601073297232E-6</v>
       </c>
+      <c r="P4" s="10"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="13">
         <v>4.8937074245143202E-6</v>
       </c>
       <c r="C5">
@@ -7709,16 +7711,17 @@
         <f t="shared" si="1"/>
         <v>-12.227560377216674</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="10">
         <f t="shared" si="0"/>
         <v>2.3476064855217493E-5</v>
       </c>
+      <c r="P5" s="10"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="13">
         <v>6.9410547272753798E-6</v>
       </c>
       <c r="C6">
@@ -7754,16 +7757,17 @@
         <f t="shared" si="1"/>
         <v>-11.878056816999475</v>
       </c>
-      <c r="O6" s="11">
+      <c r="O6" s="10">
         <f t="shared" si="0"/>
         <v>1.261241157442612E-5</v>
       </c>
+      <c r="P6" s="10"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="13">
         <v>1.39246766815199E-3</v>
       </c>
       <c r="C7">
@@ -7775,16 +7779,17 @@
         <f t="shared" si="1"/>
         <v>-6.576677804994695</v>
       </c>
-      <c r="O7" s="11">
+      <c r="O7" s="10">
         <f t="shared" si="0"/>
         <v>2.1707557752141858E-4</v>
       </c>
+      <c r="P7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="13">
         <v>1.03559232881604E-3</v>
       </c>
       <c r="C8">
@@ -7794,20 +7799,24 @@
         <f t="shared" si="1"/>
         <v>-6.8727817175920789</v>
       </c>
-      <c r="O8" s="11">
+      <c r="O8" s="10">
         <f t="shared" si="0"/>
         <v>1.4966126668337402E-4</v>
       </c>
+      <c r="P8" s="10"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="13">
         <v>2.4512692477045399E-3</v>
       </c>
       <c r="C9">
         <v>-0.57802325934675536</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
@@ -7817,11 +7826,11 @@
         <f>LN(B9)</f>
         <v>-6.0111493282848363</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="10">
         <f t="shared" si="0"/>
         <v>7.8857454756644325E-4</v>
       </c>
-      <c r="P9" s="11">
+      <c r="P9" s="10">
         <f t="shared" ref="P9:P19" si="2">EXP(K$2*C9+L$2)</f>
         <v>4.6557259463992772E-4</v>
       </c>
@@ -7830,7 +7839,7 @@
       <c r="A10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="13">
         <v>7.81250803324243E-4</v>
       </c>
       <c r="C10">
@@ -7842,11 +7851,11 @@
         <f t="shared" si="1"/>
         <v>-7.1546143286591608</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O10" s="10">
         <f t="shared" si="0"/>
         <v>7.5191856751245475E-4</v>
       </c>
-      <c r="P10" s="11">
+      <c r="P10" s="10">
         <f t="shared" si="2"/>
         <v>4.8961424901968885E-4</v>
       </c>
@@ -7855,7 +7864,7 @@
       <c r="A11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="13">
         <v>4.8135923527038E-4</v>
       </c>
       <c r="C11">
@@ -7864,18 +7873,22 @@
       <c r="D11" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E11" s="3">
-        <v>-0.04</v>
+      <c r="E11" s="4">
+        <v>-0.59058291053476397</v>
+      </c>
+      <c r="G11" s="4">
+        <f>G2*E11+H2</f>
+        <v>-7.4013632613241747</v>
       </c>
       <c r="N11" s="6">
         <f t="shared" si="1"/>
         <v>-7.6388967157388725</v>
       </c>
-      <c r="O11" s="11">
+      <c r="O11" s="10">
         <f t="shared" si="0"/>
         <v>7.5257322424679331E-4</v>
       </c>
-      <c r="P11" s="11">
+      <c r="P11" s="10">
         <f t="shared" si="2"/>
         <v>4.8916373459785382E-4</v>
       </c>
@@ -7884,7 +7897,7 @@
       <c r="A12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="13">
         <v>4.8135923527038E-4</v>
       </c>
       <c r="C12">
@@ -7892,15 +7905,19 @@
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="3"/>
+      <c r="G12" s="4">
+        <f>E11*K2+L2</f>
+        <v>-7.4013632613241747</v>
+      </c>
       <c r="N12" s="6">
         <f t="shared" si="1"/>
         <v>-7.6388967157388725</v>
       </c>
-      <c r="O12" s="11">
+      <c r="O12" s="10">
         <f t="shared" si="0"/>
         <v>7.5257322424679331E-4</v>
       </c>
-      <c r="P12" s="11">
+      <c r="P12" s="10">
         <f t="shared" si="2"/>
         <v>4.8916373459785382E-4</v>
       </c>
@@ -7909,7 +7926,7 @@
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="13">
         <v>2.5925673032070699E-4</v>
       </c>
       <c r="C13">
@@ -7917,12 +7934,16 @@
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="3"/>
+      <c r="G13" s="4">
+        <f>G12-G11</f>
+        <v>0</v>
+      </c>
       <c r="N13" s="6">
         <f t="shared" si="1"/>
         <v>-8.2576917504560008</v>
       </c>
       <c r="O13" s="10"/>
-      <c r="P13" s="11">
+      <c r="P13" s="10">
         <f t="shared" si="2"/>
         <v>4.7592454040573331E-4</v>
       </c>
@@ -7931,7 +7952,7 @@
       <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="13">
         <v>3.4869553084941298E-4</v>
       </c>
       <c r="C14">
@@ -7944,7 +7965,7 @@
         <v>-7.9613114209710165</v>
       </c>
       <c r="O14" s="10"/>
-      <c r="P14" s="11">
+      <c r="P14" s="10">
         <f t="shared" si="2"/>
         <v>1.5803734978564693E-4</v>
       </c>
@@ -7953,7 +7974,7 @@
       <c r="A15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="13">
         <v>8.0690803665655094E-6</v>
       </c>
       <c r="C15">
@@ -7968,7 +7989,7 @@
         <v>-11.727471039231094</v>
       </c>
       <c r="O15" s="10"/>
-      <c r="P15" s="11">
+      <c r="P15" s="10">
         <f t="shared" si="2"/>
         <v>4.5666846236794946E-5</v>
       </c>
@@ -7977,7 +7998,7 @@
       <c r="A16" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="13">
         <v>2.0472130855615401E-6</v>
       </c>
       <c r="C16">
@@ -7991,7 +8012,7 @@
         <v>-13.099031160190066</v>
       </c>
       <c r="O16" s="10"/>
-      <c r="P16" s="11">
+      <c r="P16" s="10">
         <f t="shared" si="2"/>
         <v>1.0465774083757679E-5</v>
       </c>
@@ -8014,7 +8035,7 @@
         <v>-15.168973904170695</v>
       </c>
       <c r="O17" s="10"/>
-      <c r="P17" s="11">
+      <c r="P17" s="10">
         <f t="shared" si="2"/>
         <v>1.2983019025165451E-7</v>
       </c>
@@ -8037,7 +8058,7 @@
         <v>-15.639814240382922</v>
       </c>
       <c r="O18" s="10"/>
-      <c r="P18" s="11">
+      <c r="P18" s="10">
         <f t="shared" si="2"/>
         <v>1.3316567797781212E-7</v>
       </c>
@@ -8061,7 +8082,7 @@
         <v>-18.073726361698615</v>
       </c>
       <c r="O19" s="10"/>
-      <c r="P19" s="11">
+      <c r="P19" s="10">
         <f t="shared" si="2"/>
         <v>1.1526279267501336E-8</v>
       </c>
@@ -8179,6 +8200,7 @@
     <mergeCell ref="J1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create correct CO2RR volcano
</commit_message>
<xml_diff>
--- a/volcanos_parsed.xlsx
+++ b/volcanos_parsed.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KTran/Google_Drive/Misc_Docs/Literature_Figures/volcanos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KTran/Google_Drive/Misc/Literature_Figures/volcanos/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="28260" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="OER" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="139">
   <si>
     <t>CoOx-(a)</t>
   </si>
@@ -170,9 +170,6 @@
     <t>RHS</t>
   </si>
   <si>
-    <t>Vertex Value</t>
-  </si>
-  <si>
     <t>E_O</t>
   </si>
   <si>
@@ -467,15 +464,44 @@
     <t>Zenith</t>
   </si>
   <si>
-    <t>x</t>
+    <t>Current density [mA/cm^2]</t>
+  </si>
+  <si>
+    <t>log(Current density [mA/cm^2])</t>
+  </si>
+  <si>
+    <t>dE_CO [eV]</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>dG, Xinyan</t>
+  </si>
+  <si>
+    <t>dE, GASpy</t>
+  </si>
+  <si>
+    <t>dG, GASpy</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>dG_CO, Xinyan [eV]</t>
+  </si>
+  <si>
+    <t>Vertex Location</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -555,7 +581,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -594,6 +620,12 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -881,11 +913,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1535015328"/>
-        <c:axId val="1449081376"/>
+        <c:axId val="-1140524592"/>
+        <c:axId val="-1217030512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1535015328"/>
+        <c:axId val="-1140524592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.4"/>
@@ -930,6 +962,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -995,13 +1028,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1449081376"/>
+        <c:crossAx val="-1217030512"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.4"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1449081376"/>
+        <c:axId val="-1217030512"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="0.85"/>
@@ -1035,6 +1068,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1101,7 +1135,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1535015328"/>
+        <c:crossAx val="-1140524592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1396,11 +1430,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1534981664"/>
-        <c:axId val="1485570176"/>
+        <c:axId val="-1140515584"/>
+        <c:axId val="-1140512464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1534981664"/>
+        <c:axId val="-1140515584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1439,6 +1473,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1504,12 +1539,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1485570176"/>
+        <c:crossAx val="-1140512464"/>
         <c:crossesAt val="-2.5"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1485570176"/>
+        <c:axId val="-1140512464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,7 +1650,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1534981664"/>
+        <c:crossAx val="-1140515584"/>
         <c:crossesAt val="-4.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2048,11 +2083,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1564948384"/>
-        <c:axId val="1564776112"/>
+        <c:axId val="-1182116416"/>
+        <c:axId val="-1182112656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1564948384"/>
+        <c:axId val="-1182116416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.8"/>
@@ -2093,6 +2128,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2158,13 +2194,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1564776112"/>
+        <c:crossAx val="-1182112656"/>
         <c:crossesAt val="1.0E-8"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.4"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1564776112"/>
+        <c:axId val="-1182112656"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2272,7 +2308,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1564948384"/>
+        <c:crossAx val="-1182116416"/>
         <c:crossesAt val="-1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2335,16 +2371,72 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Xinyan's Volcano</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.193960972269771"/>
-          <c:y val="0.0548523206751055"/>
-          <c:w val="0.726486037071453"/>
+          <c:x val="0.152723841220878"/>
+          <c:y val="0.135021097046413"/>
+          <c:w val="0.767723232405228"/>
           <c:h val="0.729817269676733"/>
         </c:manualLayout>
       </c:layout>
@@ -2470,78 +2562,704 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>CO2RR!$C$2:$C$11</c:f>
+              <c:f>CO2RR!$P$2:$P$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>-1.115386197191657</c:v>
+                  <c:v>-1.38444444444444</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.875446487125772</c:v>
+                  <c:v>-1.32222222222222</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.823324445952845</c:v>
+                  <c:v>-1.2837037037037</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.750382517993981</c:v>
+                  <c:v>-1.19185185185185</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.780854722452146</c:v>
+                  <c:v>-0.273333333333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.641291528063793</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-0.659530270571087</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.578023259346755</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.580357789932263</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-0.580315106793066</c:v>
+                  <c:v>-0.169629629629629</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>CO2RR!$B$2:$B$11</c:f>
+              <c:f>CO2RR!$B$2:$B$7</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.75900570326255E-7</c:v>
+                  <c:v>0.23444718233818</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.75680941901776E-8</c:v>
+                  <c:v>0.310159478947238</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.29118365092215E-6</c:v>
+                  <c:v>0.332367437688797</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.89370742451432E-6</c:v>
+                  <c:v>0.471333190868087</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.94105472727538E-6</c:v>
+                  <c:v>9.46370587148506</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.00139246766815199</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.00103559232881604</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.00245126924770454</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.000781250803324243</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.00048135923527038</c:v>
+                  <c:v>13.4149580158602</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.106125784909798"/>
+                  <c:y val="-0.376868002259211"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CO2RR!$P$7:$P$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>-0.169629629629629</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.177037037037036</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CO2RR!$B$7:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>13.4149580158602</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.554929385051965</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.273360349795935</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1182087824"/>
+        <c:axId val="-1182084064"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1182087824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ΔG_</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>CO (eV)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1182084064"/>
+        <c:crossesAt val="1.0E-8"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1182084064"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>j0 mA/cm2</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.023919645913826"/>
+              <c:y val="0.358895976610519"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1182087824"/>
+        <c:crossesAt val="-1.5"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>GASpy Volcano</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.152723841220878"/>
+          <c:y val="0.135021097046413"/>
+          <c:w val="0.767723232405228"/>
+          <c:h val="0.729817269676733"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0173568249620971"/>
+                  <c:y val="-0.127374663610087"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>CO2RR!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>-1.81444444444444</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.75222222222222</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.7137037037037</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.62185185185185</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.703333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.599629629629629</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>CO2RR!$B$2:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.23444718233818</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.310159478947238</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.332367437688797</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.471333190868087</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.46370587148506</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.4149580158602</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2625,72 +3343,36 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>CO2RR!$C$11:$C$19</c:f>
+              <c:f>CO2RR!$C$7:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>-0.580315106793066</c:v>
+                  <c:v>-0.599629629629629</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.580315106793066</c:v>
+                  <c:v>-0.252962962962964</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.579042912116454</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-0.527927481642916</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-0.470365711507923</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.402056089794655</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-0.19852509746354</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-0.19970125507696</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-0.086244728521156</c:v>
+                  <c:v>-0.17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>CO2RR!$B$11:$B$19</c:f>
+              <c:f>CO2RR!$B$7:$B$9</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.00048135923527038</c:v>
+                  <c:v>13.4149580158602</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00048135923527038</c:v>
+                  <c:v>0.554929385051965</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.000259256730320707</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.000348695530849413</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>8.06908036656551E-6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.04721308556154E-6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.58343974842545E-7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.61329941902728E-7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.41475218609214E-8</c:v>
+                  <c:v>0.273360349795935</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2705,15 +3387,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1528090080"/>
-        <c:axId val="1527858576"/>
+        <c:axId val="-1182044256"/>
+        <c:axId val="-1182040496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1528090080"/>
+        <c:axId val="-1182044256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.5"/>
-          <c:min val="-1.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2738,13 +3418,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>ΔG_</a:t>
+                  <a:t>ΔE_</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
                     <a:effectLst/>
                   </a:rPr>
-                  <a:t>H (eV)</a:t>
+                  <a:t>CO (eV)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -2816,17 +3496,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1527858576"/>
+        <c:crossAx val="-1182040496"/>
         <c:crossesAt val="1.0E-8"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="0.4"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1527858576"/>
+        <c:axId val="-1182040496"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
-          <c:max val="0.1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2851,7 +3529,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>j0 A/cm2</a:t>
+                  <a:t>j0 mA/cm2</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2893,7 +3571,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:numFmt formatCode="#,##0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2930,8 +3608,8 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1528090080"/>
-        <c:crossesAt val="-1.5"/>
+        <c:crossAx val="-1182044256"/>
+        <c:crossesAt val="-2.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -3139,6 +3817,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4688,6 +5406,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5317,19 +6551,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -5341,6 +6575,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5615,7 +6881,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5636,23 +6902,23 @@
         <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -5865,7 +7131,7 @@
         <v>1.5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E8" s="3">
         <f>(L2-H2)/(G2-K2)</f>
@@ -6072,7 +7338,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6087,33 +7353,33 @@
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="9">
         <v>-2.28159</v>
@@ -6152,7 +7418,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="9">
         <v>-2.0914199999999998</v>
@@ -6189,7 +7455,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="9">
         <v>-2.36334</v>
@@ -6226,7 +7492,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="9">
         <v>-1.5638000000000001</v>
@@ -6263,7 +7529,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="9">
         <v>-1.4877199999999999</v>
@@ -6300,7 +7566,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="9">
         <v>-1.3546499999999999</v>
@@ -6313,7 +7579,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="9">
         <v>-1.1404399999999999</v>
@@ -6325,7 +7591,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="9">
         <v>-1.1123799999999999</v>
@@ -6342,7 +7608,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="9">
         <v>-0.85033999999999998</v>
@@ -6359,7 +7625,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="9">
         <v>-0.56022400000000006</v>
@@ -6376,7 +7642,7 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="9">
         <v>-0.45073299999999999</v>
@@ -6385,7 +7651,7 @@
         <v>1.5826100000000001</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E12" s="3">
         <f>(L2-H2)/(G2-K2)</f>
@@ -6398,7 +7664,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="9">
         <v>-0.80348600000000003</v>
@@ -6415,7 +7681,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="9">
         <v>-1.93248</v>
@@ -6501,12 +7767,12 @@
   <dimension ref="A1:P74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="4" customWidth="1"/>
     <col min="3" max="4" width="10.83203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
@@ -6523,42 +7789,42 @@
     <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
       <c r="N1" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="13">
         <v>1.75900570326255E-7</v>
@@ -6605,7 +7871,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="13">
         <v>8.7568094190177601E-8</v>
@@ -6650,7 +7916,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <v>1.29118365092215E-6</v>
@@ -6695,7 +7961,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>4.8937074245143202E-6</v>
@@ -6740,7 +8006,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>6.9410547272753798E-6</v>
@@ -6785,7 +8051,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7">
         <v>1.39246766815199E-3</v>
@@ -6806,7 +8072,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>1.03559232881604E-3</v>
@@ -6825,7 +8091,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <v>2.4512692477045399E-3</v>
@@ -6852,7 +8118,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10">
         <v>7.81250803324243E-4</v>
@@ -6877,7 +8143,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11">
         <v>4.8135923527038E-4</v>
@@ -6886,7 +8152,7 @@
         <v>-3.0315106793066E-2</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E11" s="3">
         <v>-0.04</v>
@@ -6906,7 +8172,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12">
         <v>4.8135923527038E-4</v>
@@ -6931,7 +8197,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13">
         <v>2.5925673032070699E-4</v>
@@ -6953,7 +8219,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>3.4869553084941298E-4</v>
@@ -6975,7 +8241,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>8.0690803665655094E-6</v>
@@ -6999,7 +8265,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16">
         <v>2.0472130855615401E-6</v>
@@ -7022,7 +8288,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="13">
         <v>2.5834397484254498E-7</v>
@@ -7045,7 +8311,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="13">
         <v>1.6132994190272801E-7</v>
@@ -7068,7 +8334,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="13">
         <v>1.4147521860921401E-8</v>
@@ -7100,365 +8366,365 @@
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B65" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B67" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B68" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B69" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B70" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B71" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B72" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E73" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B74" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -7475,83 +8741,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" style="4" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="4"/>
-    <col min="7" max="7" width="16.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="8.83203125" style="4"/>
-    <col min="11" max="11" width="11.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="8.83203125" style="4"/>
-    <col min="14" max="14" width="22.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.83203125" style="4"/>
+    <col min="1" max="1" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
+      <c r="A1" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>53</v>
+        <v>131</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15" t="s">
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>127</v>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="O1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="13">
-        <v>1.75900570326255E-7</v>
-      </c>
-      <c r="C2">
-        <v>-1.115386197191657</v>
+        <v>38</v>
+      </c>
+      <c r="B2">
+        <v>0.23444718233817999</v>
+      </c>
+      <c r="C2" s="4">
+        <f>P2+AVERAGE($N$16:$O$16)</f>
+        <v>-1.8144444444444399</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="3"/>
       <c r="F2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="4">
-        <f t="array" ref="G2:H6">LINEST(N2:N12,C2:C12,TRUE,TRUE)</f>
-        <v>20.38907330959163</v>
+        <f t="array" ref="G2:H6">LINEST(O2:O7,C2:C7,TRUE,TRUE)</f>
+        <v>3.2997569714637773</v>
       </c>
       <c r="H2" s="4">
-        <v>4.6400749969611237</v>
+        <v>4.574008932663042</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>25</v>
@@ -7560,45 +8831,43 @@
         <v>19</v>
       </c>
       <c r="K2" s="4">
-        <f t="array" ref="K2:L6">LINEST(N9:N19,C9:C19,TRUE,TRUE)</f>
-        <v>-21.567419206933355</v>
+        <f t="array" ref="K2:L6">LINEST(O7:O9,C7:C9,TRUE,TRUE)</f>
+        <v>-9.0991062454081924</v>
       </c>
       <c r="L2" s="4">
-        <v>-20.138712469278246</v>
+        <v>-2.8647290301889825</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="6">
+      <c r="O2">
         <f>LN(B2)</f>
-        <v>-15.553346942875836</v>
-      </c>
-      <c r="O2" s="10">
-        <f t="shared" ref="O2:O12" si="0">EXP(G$2*C2+H$2)</f>
-        <v>1.3758404735445592E-8</v>
-      </c>
-      <c r="P2" s="10"/>
+        <v>-1.4505249516967091</v>
+      </c>
+      <c r="P2">
+        <v>-1.3844444444444399</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="13">
-        <v>8.7568094190177601E-8</v>
-      </c>
-      <c r="C3">
-        <v>-0.87544648712577211</v>
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>0.310159478947238</v>
+      </c>
+      <c r="C3" s="4">
+        <f>P3+AVERAGE($N$16:$O$16)</f>
+        <v>-1.7522222222222199</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="3"/>
       <c r="F3" s="4" t="s">
         <v>27</v>
       </c>
       <c r="G3" s="4">
-        <v>3.3929311213182962</v>
+        <v>2.4949852521757947E-2</v>
       </c>
       <c r="H3" s="4">
-        <v>2.5166510814181837</v>
+        <v>3.6418678840203778E-2</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>28</v>
@@ -7607,44 +8876,42 @@
         <v>27</v>
       </c>
       <c r="K3" s="4">
-        <v>1.8027741631968008</v>
+        <v>0.10450550171722983</v>
       </c>
       <c r="L3" s="4">
-        <v>0.8469863729200301</v>
+        <v>4.0584657137435871E-2</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="6">
-        <f t="shared" ref="N3:N19" si="1">LN(B3)</f>
-        <v>-16.250849126922169</v>
-      </c>
-      <c r="O3" s="10">
-        <f t="shared" si="0"/>
-        <v>1.8331631102289673E-6</v>
-      </c>
-      <c r="P3" s="10"/>
+      <c r="O3">
+        <f t="shared" ref="O3:O9" si="0">LN(B3)</f>
+        <v>-1.1706686655691656</v>
+      </c>
+      <c r="P3">
+        <v>-1.32222222222222</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="13">
-        <v>1.29118365092215E-6</v>
-      </c>
-      <c r="C4">
-        <v>-0.82332444595284504</v>
+        <v>43</v>
+      </c>
+      <c r="B4">
+        <v>0.33236743768879701</v>
+      </c>
+      <c r="C4" s="4">
+        <f>P4+AVERAGE($N$16:$O$16)</f>
+        <v>-1.7137037037037</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="3"/>
       <c r="F4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G4" s="4">
-        <v>0.80049409525569204</v>
+        <v>0.9997713702492429</v>
       </c>
       <c r="H4" s="4">
-        <v>1.8086039213344633</v>
+        <v>3.1192950364553645E-2</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>26</v>
@@ -7653,44 +8920,42 @@
         <v>20</v>
       </c>
       <c r="K4" s="4">
-        <v>0.94083789704750298</v>
+        <v>0.99986810645156288</v>
       </c>
       <c r="L4" s="4">
-        <v>1.0641761074450473</v>
+        <v>3.3682684131292717E-2</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="6">
-        <f t="shared" si="1"/>
-        <v>-13.559951201436114</v>
-      </c>
-      <c r="O4" s="10">
+      <c r="O4">
         <f t="shared" si="0"/>
-        <v>5.305601073297232E-6</v>
-      </c>
-      <c r="P4" s="10"/>
+        <v>-1.1015141820243972</v>
+      </c>
+      <c r="P4">
+        <v>-1.2837037037037</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="13">
-        <v>4.8937074245143202E-6</v>
-      </c>
-      <c r="C5">
-        <v>-0.75038251799398104</v>
+        <v>42</v>
+      </c>
+      <c r="B5">
+        <v>0.471333190868087</v>
+      </c>
+      <c r="C5" s="4">
+        <f>P5+AVERAGE($N$16:$O$16)</f>
+        <v>-1.6218518518518499</v>
       </c>
       <c r="D5" s="5"/>
-      <c r="E5" s="3"/>
       <c r="F5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="4">
-        <v>36.111446759105377</v>
+        <v>17491.535846730152</v>
       </c>
       <c r="H5" s="4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>24</v>
@@ -7699,44 +8964,42 @@
         <v>21</v>
       </c>
       <c r="K5" s="4">
-        <v>143.12440989845072</v>
+        <v>7580.8719857724236</v>
       </c>
       <c r="L5" s="4">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="6">
-        <f t="shared" si="1"/>
-        <v>-12.227560377216674</v>
-      </c>
-      <c r="O5" s="10">
+      <c r="O5">
         <f t="shared" si="0"/>
-        <v>2.3476064855217493E-5</v>
-      </c>
-      <c r="P5" s="10"/>
+        <v>-0.75219002345384434</v>
+      </c>
+      <c r="P5">
+        <v>-1.1918518518518499</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="13">
-        <v>6.9410547272753798E-6</v>
-      </c>
-      <c r="C6">
-        <v>-0.78085472245214604</v>
+        <v>41</v>
+      </c>
+      <c r="B6">
+        <v>9.4637058714850593</v>
+      </c>
+      <c r="C6" s="4">
+        <f>P6+AVERAGE($N$16:$O$16)</f>
+        <v>-0.70333333333333292</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="3"/>
       <c r="F6" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="4">
-        <v>118.12228090814648</v>
+        <v>17.019267045374495</v>
       </c>
       <c r="H6" s="4">
-        <v>29.439433298397581</v>
+        <v>3.8920006097820292E-3</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>23</v>
@@ -7745,453 +9008,501 @@
         <v>22</v>
       </c>
       <c r="K6" s="4">
-        <v>162.08421321062647</v>
+        <v>8.6006752220842184</v>
       </c>
       <c r="L6" s="4">
-        <v>10.192237088912034</v>
+        <v>1.1345232102884383E-3</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N6" s="6">
-        <f t="shared" si="1"/>
-        <v>-11.878056816999475</v>
-      </c>
-      <c r="O6" s="10">
+      <c r="O6">
         <f t="shared" si="0"/>
-        <v>1.261241157442612E-5</v>
-      </c>
-      <c r="P6" s="10"/>
+        <v>2.2474640475250292</v>
+      </c>
+      <c r="P6">
+        <v>-0.27333333333333298</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="13">
-        <v>1.39246766815199E-3</v>
-      </c>
-      <c r="C7">
-        <v>-0.6412915280637933</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="3"/>
-      <c r="N7" s="6">
-        <f t="shared" si="1"/>
-        <v>-6.576677804994695</v>
-      </c>
-      <c r="O7" s="10">
+        <v>128</v>
+      </c>
+      <c r="B7">
+        <v>13.414958015860201</v>
+      </c>
+      <c r="C7" s="4">
+        <f>P7+AVERAGE($N$16:$O$16)</f>
+        <v>-0.59962962962962896</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="4">
+        <f>C7</f>
+        <v>-0.59962962962962896</v>
+      </c>
+      <c r="O7">
         <f t="shared" si="0"/>
-        <v>2.1707557752141858E-4</v>
-      </c>
-      <c r="P7" s="10"/>
+        <v>2.5963703542312588</v>
+      </c>
+      <c r="P7">
+        <v>-0.16962962962962899</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="13">
-        <v>1.03559232881604E-3</v>
-      </c>
-      <c r="C8">
-        <v>-0.65953027057108704</v>
-      </c>
-      <c r="N8" s="6">
-        <f t="shared" si="1"/>
-        <v>-6.8727817175920789</v>
-      </c>
-      <c r="O8" s="10">
+        <v>45</v>
+      </c>
+      <c r="B8">
+        <v>0.55492938505196499</v>
+      </c>
+      <c r="C8" s="4">
+        <f>P8+AVERAGE($N$16:$O$16)</f>
+        <v>-0.25296296296296394</v>
+      </c>
+      <c r="O8">
         <f t="shared" si="0"/>
-        <v>1.4966126668337402E-4</v>
-      </c>
-      <c r="P8" s="10"/>
+        <v>-0.58891440747125612</v>
+      </c>
+      <c r="P8">
+        <v>0.17703703703703599</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="13">
-        <v>2.4512692477045399E-3</v>
-      </c>
-      <c r="C9">
-        <v>-0.57802325934675536</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>130</v>
+      <c r="B9">
+        <v>0.27336034979593499</v>
+      </c>
+      <c r="C9" s="4">
+        <f>P9+AVERAGE($N$16:$O$16)</f>
+        <v>-0.16999999999999993</v>
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="14"/>
       <c r="L9" s="14"/>
       <c r="M9" s="14"/>
-      <c r="N9" s="6">
-        <f>LN(B9)</f>
-        <v>-6.0111493282848363</v>
-      </c>
-      <c r="O9" s="10">
+      <c r="O9">
         <f t="shared" si="0"/>
-        <v>7.8857454756644325E-4</v>
-      </c>
-      <c r="P9" s="10">
-        <f t="shared" ref="P9:P19" si="2">EXP(K$2*C9+L$2)</f>
-        <v>4.6557259463992772E-4</v>
+        <v>-1.2969643915595344</v>
+      </c>
+      <c r="P9">
+        <v>0.26</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="13">
-        <v>7.81250803324243E-4</v>
-      </c>
-      <c r="C10">
-        <v>-0.58035778993226295</v>
-      </c>
+      <c r="A10" s="3"/>
+      <c r="B10"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="5"/>
       <c r="E10" s="3"/>
-      <c r="N10" s="6">
-        <f t="shared" si="1"/>
-        <v>-7.1546143286591608</v>
-      </c>
-      <c r="O10" s="10">
-        <f t="shared" si="0"/>
-        <v>7.5191856751245475E-4</v>
-      </c>
-      <c r="P10" s="10">
-        <f t="shared" si="2"/>
-        <v>4.8961424901968885E-4</v>
-      </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="13">
-        <v>4.8135923527038E-4</v>
-      </c>
-      <c r="C11">
-        <v>-0.58031510679306608</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E11" s="4">
-        <v>-0.59058291053476397</v>
-      </c>
-      <c r="G11" s="4">
-        <f>G2*E11+H2</f>
-        <v>-7.4013632613241747</v>
-      </c>
-      <c r="N11" s="6">
-        <f t="shared" si="1"/>
-        <v>-7.6388967157388725</v>
-      </c>
-      <c r="O11" s="10">
-        <f t="shared" si="0"/>
-        <v>7.5257322424679331E-4</v>
-      </c>
-      <c r="P11" s="10">
-        <f t="shared" si="2"/>
-        <v>4.8916373459785382E-4</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11"/>
+      <c r="C11" s="13"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="13">
-        <v>4.8135923527038E-4</v>
-      </c>
-      <c r="C12">
-        <v>-0.58031510679306608</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="5"/>
       <c r="E12" s="3"/>
-      <c r="G12" s="4">
-        <f>E11*K2+L2</f>
-        <v>-7.4013632613241747</v>
-      </c>
-      <c r="N12" s="6">
-        <f t="shared" si="1"/>
-        <v>-7.6388967157388725</v>
-      </c>
-      <c r="O12" s="10">
-        <f t="shared" si="0"/>
-        <v>7.5257322424679331E-4</v>
-      </c>
-      <c r="P12" s="10">
-        <f t="shared" si="2"/>
-        <v>4.8916373459785382E-4</v>
+      <c r="N12" s="4">
+        <v>211</v>
+      </c>
+      <c r="O12" s="4">
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="13">
-        <v>2.5925673032070699E-4</v>
-      </c>
-      <c r="C13">
-        <v>-0.57904291211645376</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="5"/>
       <c r="E13" s="3"/>
-      <c r="G13" s="4">
-        <f>G12-G11</f>
+      <c r="M13" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="N13" s="4">
+        <v>-0.27</v>
+      </c>
+      <c r="O13" s="6">
         <v>0</v>
       </c>
-      <c r="N13" s="6">
-        <f t="shared" si="1"/>
-        <v>-8.2576917504560008</v>
-      </c>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10">
-        <f t="shared" si="2"/>
-        <v>4.7592454040573331E-4</v>
-      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="13">
-        <v>3.4869553084941298E-4</v>
-      </c>
-      <c r="C14">
-        <v>-0.5279274816429157</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="5"/>
       <c r="E14" s="3"/>
-      <c r="N14" s="6">
-        <f t="shared" si="1"/>
-        <v>-7.9613114209710165</v>
-      </c>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10">
-        <f t="shared" si="2"/>
-        <v>1.5803734978564693E-4</v>
-      </c>
+      <c r="G14" s="15"/>
+      <c r="M14" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="N14" s="4">
+        <v>-0.69</v>
+      </c>
+      <c r="O14" s="6">
+        <v>-0.44</v>
+      </c>
+      <c r="P14" s="6"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="13">
-        <v>8.0690803665655094E-6</v>
-      </c>
-      <c r="C15">
-        <v>-0.47036571150792272</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="5"/>
       <c r="E15" s="3"/>
       <c r="H15" s="6"/>
       <c r="L15" s="6"/>
-      <c r="N15" s="6">
-        <f>LN(B15)</f>
-        <v>-11.727471039231094</v>
-      </c>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10">
-        <f t="shared" si="2"/>
-        <v>4.5666846236794946E-5</v>
-      </c>
+      <c r="M15" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="N15" s="4">
+        <f>N14+0.54</f>
+        <v>-0.14999999999999991</v>
+      </c>
+      <c r="O15" s="6">
+        <f>O14+0.54</f>
+        <v>0.10000000000000003</v>
+      </c>
+      <c r="P15" s="6"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="13">
-        <v>2.0472130855615401E-6</v>
-      </c>
-      <c r="C16">
-        <v>-0.40205608979465501</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16"/>
+      <c r="C16" s="13"/>
       <c r="D16" s="5"/>
       <c r="E16" s="3"/>
       <c r="L16" s="6"/>
-      <c r="N16" s="6">
-        <f t="shared" si="1"/>
-        <v>-13.099031160190066</v>
-      </c>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10">
-        <f t="shared" si="2"/>
-        <v>1.0465774083757679E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="13">
-        <v>2.5834397484254498E-7</v>
-      </c>
-      <c r="C17">
-        <v>-0.19852509746354002</v>
-      </c>
+      <c r="M16" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N16" s="4">
+        <f>N14-N13</f>
+        <v>-0.41999999999999993</v>
+      </c>
+      <c r="O16" s="4">
+        <f>O14-O13</f>
+        <v>-0.44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17"/>
+      <c r="C17" s="13"/>
       <c r="D17" s="5"/>
       <c r="E17" s="3"/>
+      <c r="G17" s="15"/>
       <c r="L17" s="6"/>
-      <c r="N17" s="6">
-        <f t="shared" si="1"/>
-        <v>-15.168973904170695</v>
-      </c>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10">
-        <f t="shared" si="2"/>
-        <v>1.2983019025165451E-7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="13">
-        <v>1.6132994190272801E-7</v>
-      </c>
-      <c r="C18">
-        <v>-0.19970125507696007</v>
-      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18"/>
+      <c r="C18" s="13"/>
       <c r="D18" s="5"/>
       <c r="E18" s="3"/>
       <c r="L18" s="6"/>
-      <c r="N18" s="6">
-        <f t="shared" si="1"/>
-        <v>-15.639814240382922</v>
-      </c>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10">
-        <f t="shared" si="2"/>
-        <v>1.3316567797781212E-7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="13">
-        <v>1.4147521860921401E-8</v>
-      </c>
-      <c r="C19">
-        <v>-8.6244728521156055E-2</v>
-      </c>
+      <c r="M18" s="4">
+        <f>EXP(C2*G$2+H$2)</f>
+        <v>0.24335919161903002</v>
+      </c>
+      <c r="N18"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B19"/>
+      <c r="C19" s="13"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="H19" s="7"/>
       <c r="L19" s="6"/>
-      <c r="N19" s="6">
-        <f t="shared" si="1"/>
-        <v>-18.073726361698615</v>
-      </c>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10">
-        <f t="shared" si="2"/>
-        <v>1.1526279267501336E-8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="N20" s="6"/>
-      <c r="O20" s="10"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M19" s="4">
+        <f>EXP(C3*G$2+H$2)</f>
+        <v>0.29882458180953059</v>
+      </c>
+      <c r="N19"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M20" s="4">
+        <f>EXP(C4*G$2+H$2)</f>
+        <v>0.33932504008839076</v>
+      </c>
+      <c r="N20"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G21" s="11"/>
       <c r="K21" s="6"/>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="M21" s="4">
+        <f>EXP(C5*G$2+H$2)</f>
+        <v>0.45945787268287569</v>
+      </c>
+      <c r="N21"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M22" s="4">
+        <f>EXP(C6*G$2+H$2)</f>
+        <v>9.5179535526026662</v>
+      </c>
+      <c r="N22"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M23" s="4">
+        <f>EXP(C7*G$2+H$2)</f>
+        <v>13.401637245543412</v>
+      </c>
+      <c r="N23">
+        <f>EXP(C7*K$2+L$2)</f>
+        <v>13.347974863292285</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N24">
+        <f>EXP(C8*K$2+L$2)</f>
+        <v>0.56950247280807387</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N25">
+        <f>EXP(C9*K$2+L$2)</f>
+        <v>0.26770197027556697</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N26"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="3"/>
+      <c r="E34" s="15"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D42" s="4" t="s">
+        <v>89</v>
+      </c>
       <c r="E42" s="12"/>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D43" s="4" t="s">
+        <v>90</v>
+      </c>
       <c r="E43" s="12"/>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D44" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="E44" s="12"/>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D45" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="E45" s="12"/>
     </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D46" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="E46" s="12"/>
     </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D47" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="E47" s="12"/>
     </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D48" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="E48" s="12"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D49" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="E49" s="12"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D50" s="4" t="s">
+        <v>97</v>
+      </c>
       <c r="E50" s="12"/>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D51" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="E51" s="12"/>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D52" s="4" t="s">
+        <v>98</v>
+      </c>
       <c r="E52" s="12"/>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D53" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="E53" s="12"/>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D54" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="E54" s="12"/>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D55" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="E55" s="12"/>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D56" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="E56" s="12"/>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D57" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="E57" s="12"/>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D58" s="4" t="s">
+        <v>102</v>
+      </c>
       <c r="E58" s="12"/>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D59" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="E59" s="12"/>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D60" s="4" t="s">
+        <v>104</v>
+      </c>
       <c r="E60" s="12"/>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D61" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="E61" s="12"/>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D62" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="E62" s="12"/>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D63" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="E63" s="12"/>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D64" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="E64" s="12"/>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D65" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="E65" s="12"/>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D66" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="E66" s="12"/>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D67" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="E67" s="12"/>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D68" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="E68" s="12"/>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D69" s="4" t="s">
+        <v>95</v>
+      </c>
       <c r="E69" s="12"/>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D70" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="E70" s="12"/>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D71" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="E71" s="12"/>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D72" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="E72" s="12"/>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D73" s="4" t="s">
+        <v>87</v>
+      </c>
       <c r="E73" s="12"/>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D74" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="E74" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add HER and Google Drive dumping
</commit_message>
<xml_diff>
--- a/volcanos_parsed.xlsx
+++ b/volcanos_parsed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OER" sheetId="1" r:id="rId1"/>
@@ -230,12 +230,6 @@
     <t>Au(111)</t>
   </si>
   <si>
-    <t>Transformed current density</t>
-  </si>
-  <si>
-    <t>dG_H [eV]</t>
-  </si>
-  <si>
     <t>Current density [A/cm^2]</t>
   </si>
   <si>
@@ -455,9 +449,6 @@
     <t>(010)</t>
   </si>
   <si>
-    <t>Double-check model (LHS)</t>
-  </si>
-  <si>
     <t>Zenith?</t>
   </si>
   <si>
@@ -492,6 +483,15 @@
   </si>
   <si>
     <t>Vertex Location</t>
+  </si>
+  <si>
+    <t>log(Current density [A/cm^2])</t>
+  </si>
+  <si>
+    <t>Experimental dG_H [eV]</t>
+  </si>
+  <si>
+    <t>dE_H [eV]</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -608,9 +608,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -913,11 +910,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1140524592"/>
-        <c:axId val="-1217030512"/>
+        <c:axId val="-891165872"/>
+        <c:axId val="-894012448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1140524592"/>
+        <c:axId val="-891165872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2.4"/>
@@ -962,7 +959,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1028,13 +1024,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1217030512"/>
+        <c:crossAx val="-894012448"/>
         <c:crossesAt val="0.0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.4"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1217030512"/>
+        <c:axId val="-894012448"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="0.85"/>
@@ -1068,7 +1064,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1135,7 +1130,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1140524592"/>
+        <c:crossAx val="-891165872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1430,11 +1425,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1140515584"/>
-        <c:axId val="-1140512464"/>
+        <c:axId val="-891145872"/>
+        <c:axId val="-891142480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1140515584"/>
+        <c:axId val="-891145872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1473,7 +1468,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1539,12 +1533,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1140512464"/>
+        <c:crossAx val="-891142480"/>
         <c:crossesAt val="-2.5"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1140512464"/>
+        <c:axId val="-891142480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1650,7 +1644,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1140515584"/>
+        <c:crossAx val="-891145872"/>
         <c:crossesAt val="-4.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1713,15 +1707,785 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Experimental Volcano</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.193960972269771"/>
-          <c:y val="0.0548523206751055"/>
+          <c:x val="0.176954041459103"/>
+          <c:y val="0.130801687763713"/>
+          <c:w val="0.726486037071453"/>
+          <c:h val="0.729817269676733"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0173568249620971"/>
+                  <c:y val="-0.127374663610087"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>HER!$O$2:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-0.565386197191657</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.325446487125772</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.273324445952845</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.200382517993981</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.230854722452146</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.0912915280637933</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.109530270571087</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.0280232593467553</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.0303577899322629</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.030315106793066</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>HER!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.75900570326255E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.75680941901776E-8</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>1.29118365092215E-6</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>4.89370742451432E-6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>6.94105472727538E-6</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.00139246766815199</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.00103559232881604</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>0.00245126924770454</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>0.000781250803324243</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>0.00048135923527038</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0798620824570842"/>
+                  <c:y val="-0.36677464367587"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>HER!$O$11:$O$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>-0.030315106793066</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.030315106793066</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.0290429121164537</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0220725183570844</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0796342884920773</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.147943910205345</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.35147490253646</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35029874492304</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.463755271478844</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>HER!$B$11:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.00048135923527038</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00048135923527038</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.000259256730320707</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000348695530849413</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.06908036656551E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.04721308556154E-6</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="0.00E+00">
+                  <c:v>2.58343974842545E-7</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="0.00E+00">
+                  <c:v>1.61329941902728E-7</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="0.00E+00">
+                  <c:v>1.41475218609214E-8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-891097280"/>
+        <c:axId val="-891093520"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-891097280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.8"/>
+          <c:min val="-0.8"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>ΔG_</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>H (eV)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-891093520"/>
+        <c:crossesAt val="1.0E-8"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="0.4"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-891093520"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+          <c:max val="0.1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>j0 A/cm2</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.023919645913826"/>
+              <c:y val="0.358895976610519"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.E+00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-891097280"/>
+        <c:crossesAt val="-1.0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>GASpy Volcano</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.173552680914886"/>
+          <c:y val="0.139240506329114"/>
           <c:w val="0.726486037071453"/>
           <c:h val="0.729817269676733"/>
         </c:manualLayout>
@@ -1853,34 +2617,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-0.565386197191657</c:v>
+                  <c:v>-0.805386197191657</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.325446487125772</c:v>
+                  <c:v>-0.565446487125772</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.273324445952845</c:v>
+                  <c:v>-0.513324445952845</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.200382517993981</c:v>
+                  <c:v>-0.440382517993981</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.230854722452146</c:v>
+                  <c:v>-0.470854722452146</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.0912915280637933</c:v>
+                  <c:v>-0.331291528063793</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.109530270571087</c:v>
+                  <c:v>-0.349530270571087</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.0280232593467553</c:v>
+                  <c:v>-0.268023259346755</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.0303577899322629</c:v>
+                  <c:v>-0.270357789932263</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.030315106793066</c:v>
+                  <c:v>-0.270315106793066</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2008,31 +2772,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-0.030315106793066</c:v>
+                  <c:v>-0.270315106793066</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.030315106793066</c:v>
+                  <c:v>-0.270315106793066</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.0290429121164537</c:v>
+                  <c:v>-0.269042912116454</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0220725183570844</c:v>
+                  <c:v>-0.217927481642916</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0796342884920773</c:v>
+                  <c:v>-0.160365711507923</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.147943910205345</c:v>
+                  <c:v>-0.092056089794655</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.35147490253646</c:v>
+                  <c:v>0.11147490253646</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.35029874492304</c:v>
+                  <c:v>0.11029874492304</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.463755271478844</c:v>
+                  <c:v>0.223755271478844</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2083,15 +2847,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1182116416"/>
-        <c:axId val="-1182112656"/>
+        <c:axId val="-973687040"/>
+        <c:axId val="-973683280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1182116416"/>
+        <c:axId val="-973687040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.8"/>
-          <c:min val="-0.8"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2116,7 +2878,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>ΔG_</a:t>
+                  <a:t>ΔE_</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
@@ -2194,13 +2956,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1182112656"/>
+        <c:crossAx val="-973683280"/>
         <c:crossesAt val="1.0E-8"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.4"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1182112656"/>
+        <c:axId val="-973683280"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2308,7 +3070,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1182116416"/>
+        <c:crossAx val="-973687040"/>
         <c:crossesAt val="-1.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2357,7 +3119,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2737,11 +3499,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1182087824"/>
-        <c:axId val="-1182084064"/>
+        <c:axId val="-893963008"/>
+        <c:axId val="-893959248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1182087824"/>
+        <c:axId val="-893963008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2846,12 +3608,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1182084064"/>
+        <c:crossAx val="-893959248"/>
         <c:crossesAt val="1.0E-8"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1182084064"/>
+        <c:axId val="-893959248"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2958,7 +3720,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1182087824"/>
+        <c:crossAx val="-893963008"/>
         <c:crossesAt val="-1.5"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3007,7 +3769,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3387,11 +4149,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1182044256"/>
-        <c:axId val="-1182040496"/>
+        <c:axId val="-893934000"/>
+        <c:axId val="-893930240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1182044256"/>
+        <c:axId val="-893934000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3496,12 +4258,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1182040496"/>
+        <c:crossAx val="-893930240"/>
         <c:crossesAt val="1.0E-8"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1182040496"/>
+        <c:axId val="-893930240"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3608,7 +4370,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1182044256"/>
+        <c:crossAx val="-893934000"/>
         <c:crossesAt val="-2.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3857,6 +4619,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5922,6 +6724,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6513,16 +7831,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6543,6 +7861,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6550,16 +7900,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6582,16 +7932,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6902,23 +8252,23 @@
         <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -7131,7 +8481,7 @@
         <v>1.5</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E8" s="3">
         <f>(L2-H2)/(G2-K2)</f>
@@ -7359,23 +8709,23 @@
         <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -7651,7 +9001,7 @@
         <v>1.5826100000000001</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E12" s="3">
         <f>(L2-H2)/(G2-K2)</f>
@@ -7764,15 +9114,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P74"/>
+  <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="4" customWidth="1"/>
     <col min="3" max="4" width="10.83203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
@@ -7782,55 +9132,55 @@
     <col min="11" max="11" width="11.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="8.83203125" style="4"/>
     <col min="14" max="14" width="22.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.83203125" style="4"/>
+    <col min="15" max="15" width="11.1640625" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
+    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>129</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>52</v>
+        <v>138</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="12">
         <v>1.75900570326255E-7</v>
       </c>
-      <c r="C2">
-        <v>-0.56538619719165695</v>
+      <c r="C2" s="4">
+        <f>O2-0.24</f>
+        <v>-0.80538619719165694</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="3"/>
@@ -7839,10 +9189,10 @@
       </c>
       <c r="G2" s="4">
         <f t="array" ref="G2:H6">LINEST(N2:N12,C2:C12,TRUE,TRUE)</f>
-        <v>20.38907330959163</v>
+        <v>20.389073309591609</v>
       </c>
       <c r="H2" s="4">
-        <v>-6.5739153233142744</v>
+        <v>-1.6805377290122898</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>25</v>
@@ -7852,10 +9202,10 @@
       </c>
       <c r="K2" s="4">
         <f t="array" ref="K2:L6">LINEST(N9:N19,C9:C19,TRUE,TRUE)</f>
-        <v>-21.567419206933351</v>
+        <v>-21.567419206933359</v>
       </c>
       <c r="L2" s="4">
-        <v>-8.2766319054649014</v>
+        <v>-13.452812515128906</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>25</v>
@@ -7864,20 +9214,20 @@
         <f>LN(B2)</f>
         <v>-15.553346942875836</v>
       </c>
-      <c r="O2" s="11">
-        <f t="shared" ref="O2:O12" si="0">EXP(G$2*C2+H$2)</f>
-        <v>1.3758404735445592E-8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O2">
+        <v>-0.56538619719165695</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="12">
         <v>8.7568094190177601E-8</v>
       </c>
-      <c r="C3">
-        <v>-0.32544648712577201</v>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:C19" si="0">O3-0.24</f>
+        <v>-0.56544648712577206</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="3"/>
@@ -7885,10 +9235,10 @@
         <v>27</v>
       </c>
       <c r="G3" s="4">
-        <v>3.3929311213182967</v>
+        <v>3.392931121318294</v>
       </c>
       <c r="H3" s="4">
-        <v>0.80396015984208757</v>
+        <v>1.5071626888645753</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>28</v>
@@ -7897,10 +9247,10 @@
         <v>27</v>
       </c>
       <c r="K3" s="4">
-        <v>1.8027741631968017</v>
+        <v>1.8027741631968019</v>
       </c>
       <c r="L3" s="4">
-        <v>0.38220102736211103</v>
+        <v>0.39188797383178398</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>28</v>
@@ -7909,20 +9259,20 @@
         <f t="shared" ref="N3:N19" si="1">LN(B3)</f>
         <v>-16.250849126922169</v>
       </c>
-      <c r="O3" s="11">
-        <f t="shared" si="0"/>
-        <v>1.8331631102289673E-6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O3">
+        <v>-0.32544648712577201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B4">
         <v>1.29118365092215E-6</v>
       </c>
-      <c r="C4">
-        <v>-0.273324445952845</v>
+      <c r="C4" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.51332444595284499</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="3"/>
@@ -7930,10 +9280,10 @@
         <v>20</v>
       </c>
       <c r="G4" s="4">
-        <v>0.80049409525569193</v>
+        <v>0.80049409525569204</v>
       </c>
       <c r="H4" s="4">
-        <v>1.8086039213344636</v>
+        <v>1.8086039213344631</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>26</v>
@@ -7945,7 +9295,7 @@
         <v>0.94083789704750298</v>
       </c>
       <c r="L4" s="4">
-        <v>1.0641761074450475</v>
+        <v>1.0641761074450478</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>26</v>
@@ -7954,20 +9304,20 @@
         <f t="shared" si="1"/>
         <v>-13.559951201436114</v>
       </c>
-      <c r="O4" s="11">
-        <f t="shared" si="0"/>
-        <v>5.3056010732972226E-6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O4">
+        <v>-0.273324445952845</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B5">
         <v>4.8937074245143202E-6</v>
       </c>
-      <c r="C5">
-        <v>-0.20038251799398099</v>
+      <c r="C5" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.44038251799398098</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="3"/>
@@ -7975,7 +9325,7 @@
         <v>21</v>
       </c>
       <c r="G5" s="4">
-        <v>36.111446759105363</v>
+        <v>36.111446759105391</v>
       </c>
       <c r="H5" s="4">
         <v>9</v>
@@ -7987,7 +9337,7 @@
         <v>21</v>
       </c>
       <c r="K5" s="4">
-        <v>143.12440989845064</v>
+        <v>143.12440989845061</v>
       </c>
       <c r="L5" s="4">
         <v>9</v>
@@ -7999,20 +9349,20 @@
         <f t="shared" si="1"/>
         <v>-12.227560377216674</v>
       </c>
-      <c r="O5" s="11">
-        <f t="shared" si="0"/>
-        <v>2.3476064855217453E-5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O5">
+        <v>-0.20038251799398099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B6">
         <v>6.9410547272753798E-6</v>
       </c>
-      <c r="C6">
-        <v>-0.230854722452146</v>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.47085472245214599</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="3"/>
@@ -8020,10 +9370,10 @@
         <v>22</v>
       </c>
       <c r="G6" s="4">
-        <v>118.12228090814646</v>
+        <v>118.12228090814648</v>
       </c>
       <c r="H6" s="4">
-        <v>29.439433298397589</v>
+        <v>29.439433298397567</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>23</v>
@@ -8035,7 +9385,7 @@
         <v>162.08421321062647</v>
       </c>
       <c r="L6" s="4">
-        <v>10.192237088912043</v>
+        <v>10.192237088912044</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>23</v>
@@ -8044,20 +9394,20 @@
         <f t="shared" si="1"/>
         <v>-11.878056816999475</v>
       </c>
-      <c r="O6" s="11">
-        <f t="shared" si="0"/>
-        <v>1.261241157442612E-5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O6">
+        <v>-0.230854722452146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B7">
         <v>1.39246766815199E-3</v>
       </c>
-      <c r="C7">
-        <v>-9.1291528063793301E-2</v>
+      <c r="C7" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.33129152806379331</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="3"/>
@@ -8065,39 +9415,39 @@
         <f t="shared" si="1"/>
         <v>-6.576677804994695</v>
       </c>
-      <c r="O7" s="11">
-        <f t="shared" si="0"/>
-        <v>2.170755775214182E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>-9.1291528063793301E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B8">
         <v>1.03559232881604E-3</v>
       </c>
-      <c r="C8">
-        <v>-0.109530270571087</v>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.34953027057108699</v>
       </c>
       <c r="N8" s="6">
         <f t="shared" si="1"/>
         <v>-6.8727817175920789</v>
       </c>
-      <c r="O8" s="11">
-        <f t="shared" si="0"/>
-        <v>1.4966126668337402E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>-0.109530270571087</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B9">
         <v>2.4512692477045399E-3</v>
       </c>
-      <c r="C9">
-        <v>-2.80232593467553E-2</v>
+      <c r="C9" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.2680232593467553</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -8107,24 +9457,20 @@
         <f>LN(B9)</f>
         <v>-6.0111493282848363</v>
       </c>
-      <c r="O9" s="11">
-        <f t="shared" si="0"/>
-        <v>7.8857454756644325E-4</v>
-      </c>
-      <c r="P9" s="11">
-        <f t="shared" ref="P9:P19" si="2">EXP(K$2*C9+L$2)</f>
-        <v>4.6557259463992728E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <v>-2.80232593467553E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B10">
         <v>7.81250803324243E-4</v>
       </c>
-      <c r="C10">
-        <v>-3.0357789932262898E-2</v>
+      <c r="C10" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.27035778993226289</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="3"/>
@@ -8132,53 +9478,45 @@
         <f t="shared" si="1"/>
         <v>-7.1546143286591608</v>
       </c>
-      <c r="O10" s="11">
-        <f t="shared" si="0"/>
-        <v>7.519185675124541E-4</v>
-      </c>
-      <c r="P10" s="11">
-        <f t="shared" si="2"/>
-        <v>4.8961424901968842E-4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O10">
+        <v>-3.0357789932262898E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B11">
         <v>4.8135923527038E-4</v>
       </c>
-      <c r="C11">
-        <v>-3.0315106793066E-2</v>
+      <c r="C11" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.27031510679306597</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E11" s="3">
-        <v>-0.04</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="N11" s="6">
         <f t="shared" si="1"/>
         <v>-7.6388967157388725</v>
       </c>
-      <c r="O11" s="11">
-        <f t="shared" si="0"/>
-        <v>7.5257322424679331E-4</v>
-      </c>
-      <c r="P11" s="11">
-        <f t="shared" si="2"/>
-        <v>4.8916373459785252E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <v>-3.0315106793066E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B12">
         <v>4.8135923527038E-4</v>
       </c>
-      <c r="C12">
-        <v>-3.0315106793066E-2</v>
+      <c r="C12" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.27031510679306597</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="3"/>
@@ -8186,24 +9524,20 @@
         <f t="shared" si="1"/>
         <v>-7.6388967157388725</v>
       </c>
-      <c r="O12" s="11">
-        <f t="shared" si="0"/>
-        <v>7.5257322424679331E-4</v>
-      </c>
-      <c r="P12" s="11">
-        <f t="shared" si="2"/>
-        <v>4.8916373459785252E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O12">
+        <v>-3.0315106793066E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B13">
         <v>2.5925673032070699E-4</v>
       </c>
-      <c r="C13">
-        <v>-2.9042912116453701E-2</v>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.2690429121164537</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="3"/>
@@ -8211,21 +9545,20 @@
         <f t="shared" si="1"/>
         <v>-8.2576917504560008</v>
       </c>
-      <c r="O13" s="10"/>
-      <c r="P13" s="11">
-        <f t="shared" si="2"/>
-        <v>4.7592454040573206E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O13">
+        <v>-2.9042912116453701E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B14">
         <v>3.4869553084941298E-4</v>
       </c>
-      <c r="C14">
-        <v>2.20725183570844E-2</v>
+      <c r="C14" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.21792748164291559</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="3"/>
@@ -8233,21 +9566,20 @@
         <f t="shared" si="1"/>
         <v>-7.9613114209710165</v>
       </c>
-      <c r="O14" s="10"/>
-      <c r="P14" s="11">
-        <f t="shared" si="2"/>
-        <v>1.5803734978564663E-4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O14">
+        <v>2.20725183570844E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B15">
         <v>8.0690803665655094E-6</v>
       </c>
-      <c r="C15">
-        <v>7.9634288492077293E-2</v>
+      <c r="C15" s="4">
+        <f t="shared" si="0"/>
+        <v>-0.1603657115079227</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="3"/>
@@ -8257,21 +9589,20 @@
         <f>LN(B15)</f>
         <v>-11.727471039231094</v>
       </c>
-      <c r="O15" s="10"/>
-      <c r="P15" s="11">
-        <f t="shared" si="2"/>
-        <v>4.5666846236794946E-5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O15">
+        <v>7.9634288492077293E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B16">
         <v>2.0472130855615401E-6</v>
       </c>
-      <c r="C16">
-        <v>0.147943910205345</v>
+      <c r="C16" s="4">
+        <f t="shared" si="0"/>
+        <v>-9.2056089794654988E-2</v>
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="3"/>
@@ -8280,21 +9611,20 @@
         <f t="shared" si="1"/>
         <v>-13.099031160190066</v>
       </c>
-      <c r="O16" s="10"/>
-      <c r="P16" s="11">
-        <f t="shared" si="2"/>
-        <v>1.0465774083757679E-5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O16">
+        <v>0.147943910205345</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="12">
         <v>2.5834397484254498E-7</v>
       </c>
-      <c r="C17">
-        <v>0.35147490253646002</v>
+      <c r="C17" s="4">
+        <f t="shared" si="0"/>
+        <v>0.11147490253646003</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="3"/>
@@ -8303,21 +9633,20 @@
         <f t="shared" si="1"/>
         <v>-15.168973904170695</v>
       </c>
-      <c r="O17" s="10"/>
-      <c r="P17" s="11">
-        <f t="shared" si="2"/>
-        <v>1.2983019025165473E-7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O17">
+        <v>0.35147490253646002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="12">
         <v>1.6132994190272801E-7</v>
       </c>
-      <c r="C18">
-        <v>0.35029874492303997</v>
+      <c r="C18" s="4">
+        <f t="shared" si="0"/>
+        <v>0.11029874492303998</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="3"/>
@@ -8326,21 +9655,20 @@
         <f t="shared" si="1"/>
         <v>-15.639814240382922</v>
       </c>
-      <c r="O18" s="10"/>
-      <c r="P18" s="11">
-        <f t="shared" si="2"/>
-        <v>1.3316567797781212E-7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O18">
+        <v>0.35029874492303997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="12">
         <v>1.4147521860921401E-8</v>
       </c>
-      <c r="C19">
-        <v>0.46375527147884399</v>
+      <c r="C19" s="4">
+        <f t="shared" si="0"/>
+        <v>0.223755271478844</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -8350,381 +9678,378 @@
         <f t="shared" si="1"/>
         <v>-18.073726361698615</v>
       </c>
-      <c r="O19" s="10"/>
-      <c r="P19" s="11">
-        <f t="shared" si="2"/>
-        <v>1.1526279267501336E-8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O19">
+        <v>0.46375527147884399</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="N20" s="6"/>
-      <c r="O20" s="10"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="G21" s="11"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G21" s="10"/>
       <c r="K21" s="6"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>117</v>
+        <v>87</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>118</v>
+        <v>88</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>119</v>
+        <v>89</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>118</v>
+        <v>90</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>117</v>
+        <v>91</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>120</v>
+        <v>92</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>118</v>
+        <v>93</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>121</v>
+        <v>94</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B50" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>118</v>
+        <v>95</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>122</v>
+        <v>85</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>123</v>
+        <v>96</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B53" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>117</v>
+        <v>86</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B54" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>120</v>
+        <v>93</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B55" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>117</v>
+        <v>97</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B56" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>117</v>
+        <v>98</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E57" s="12" t="s">
-        <v>120</v>
+        <v>99</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B58" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E58" s="12" t="s">
-        <v>124</v>
+        <v>100</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B59" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>121</v>
+        <v>101</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>117</v>
+        <v>102</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B61" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E61" s="12" t="s">
-        <v>122</v>
+        <v>103</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B62" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E62" s="12" t="s">
-        <v>121</v>
+        <v>104</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B63" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>117</v>
+        <v>105</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B64" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>120</v>
+        <v>106</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B65" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E65" s="12" t="s">
-        <v>125</v>
+        <v>107</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E66" s="12" t="s">
-        <v>116</v>
+        <v>108</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B67" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E67" s="12" t="s">
-        <v>117</v>
+        <v>109</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B68" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E68" s="12" t="s">
-        <v>121</v>
+        <v>110</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B69" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>124</v>
+        <v>93</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B70" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E70" s="12" t="s">
-        <v>120</v>
+        <v>111</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B71" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E71" s="12" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B72" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E72" s="12" t="s">
-        <v>118</v>
+        <v>113</v>
+      </c>
+      <c r="E72" s="11" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="73" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B73" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D73" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D73" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E73" s="12" t="s">
-        <v>121</v>
+      <c r="E73" s="11" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B74" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E74" s="12" t="s">
-        <v>118</v>
+        <v>103</v>
+      </c>
+      <c r="E74" s="11" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -8741,8 +10066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8769,37 +10094,37 @@
   <sheetData>
     <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="O1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="O1" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="P1" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -8856,7 +10181,7 @@
         <v>0.310159478947238</v>
       </c>
       <c r="C3" s="4">
-        <f>P3+AVERAGE($N$16:$O$16)</f>
+        <f t="shared" ref="C3:C9" si="0">P3+AVERAGE($N$16:$O$16)</f>
         <v>-1.7522222222222199</v>
       </c>
       <c r="D3" s="5"/>
@@ -8885,7 +10210,7 @@
         <v>28</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O9" si="0">LN(B3)</f>
+        <f t="shared" ref="O3:O9" si="1">LN(B3)</f>
         <v>-1.1706686655691656</v>
       </c>
       <c r="P3">
@@ -8900,7 +10225,7 @@
         <v>0.33236743768879701</v>
       </c>
       <c r="C4" s="4">
-        <f>P4+AVERAGE($N$16:$O$16)</f>
+        <f t="shared" si="0"/>
         <v>-1.7137037037037</v>
       </c>
       <c r="D4" s="5"/>
@@ -8929,7 +10254,7 @@
         <v>26</v>
       </c>
       <c r="O4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.1015141820243972</v>
       </c>
       <c r="P4">
@@ -8944,7 +10269,7 @@
         <v>0.471333190868087</v>
       </c>
       <c r="C5" s="4">
-        <f>P5+AVERAGE($N$16:$O$16)</f>
+        <f t="shared" si="0"/>
         <v>-1.6218518518518499</v>
       </c>
       <c r="D5" s="5"/>
@@ -8973,7 +10298,7 @@
         <v>24</v>
       </c>
       <c r="O5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.75219002345384434</v>
       </c>
       <c r="P5">
@@ -8988,7 +10313,7 @@
         <v>9.4637058714850593</v>
       </c>
       <c r="C6" s="4">
-        <f>P6+AVERAGE($N$16:$O$16)</f>
+        <f t="shared" si="0"/>
         <v>-0.70333333333333292</v>
       </c>
       <c r="D6" s="5"/>
@@ -9017,7 +10342,7 @@
         <v>23</v>
       </c>
       <c r="O6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2474640475250292</v>
       </c>
       <c r="P6">
@@ -9026,24 +10351,24 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B7">
         <v>13.414958015860201</v>
       </c>
       <c r="C7" s="4">
-        <f>P7+AVERAGE($N$16:$O$16)</f>
+        <f t="shared" si="0"/>
         <v>-0.59962962962962896</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E7" s="4">
         <f>C7</f>
         <v>-0.59962962962962896</v>
       </c>
       <c r="O7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.5963703542312588</v>
       </c>
       <c r="P7">
@@ -9058,11 +10383,11 @@
         <v>0.55492938505196499</v>
       </c>
       <c r="C8" s="4">
-        <f>P8+AVERAGE($N$16:$O$16)</f>
+        <f t="shared" si="0"/>
         <v>-0.25296296296296394</v>
       </c>
       <c r="O8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-0.58891440747125612</v>
       </c>
       <c r="P8">
@@ -9077,15 +10402,15 @@
         <v>0.27336034979593499</v>
       </c>
       <c r="C9" s="4">
-        <f>P9+AVERAGE($N$16:$O$16)</f>
+        <f t="shared" si="0"/>
         <v>-0.16999999999999993</v>
       </c>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
       <c r="O9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.2969643915595344</v>
       </c>
       <c r="P9">
@@ -9095,19 +10420,19 @@
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10"/>
-      <c r="C10" s="13"/>
+      <c r="C10" s="12"/>
       <c r="D10" s="5"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11"/>
-      <c r="C11" s="13"/>
+      <c r="C11" s="12"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12"/>
-      <c r="C12" s="13"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="5"/>
       <c r="E12" s="3"/>
       <c r="N12" s="4">
@@ -9120,11 +10445,11 @@
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13"/>
-      <c r="C13" s="13"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="5"/>
       <c r="E13" s="3"/>
       <c r="M13" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="N13" s="4">
         <v>-0.27</v>
@@ -9136,12 +10461,12 @@
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14"/>
-      <c r="C14" s="13"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="5"/>
       <c r="E14" s="3"/>
-      <c r="G14" s="15"/>
-      <c r="M14" s="16" t="s">
-        <v>134</v>
+      <c r="G14" s="14"/>
+      <c r="M14" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="N14" s="4">
         <v>-0.69</v>
@@ -9154,13 +10479,13 @@
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15"/>
-      <c r="C15" s="13"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="5"/>
       <c r="E15" s="3"/>
       <c r="H15" s="6"/>
       <c r="L15" s="6"/>
       <c r="M15" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N15" s="4">
         <f>N14+0.54</f>
@@ -9175,12 +10500,12 @@
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16"/>
-      <c r="C16" s="13"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="5"/>
       <c r="E16" s="3"/>
       <c r="L16" s="6"/>
       <c r="M16" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="N16" s="4">
         <f>N14-N13</f>
@@ -9194,63 +10519,63 @@
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17"/>
-      <c r="C17" s="13"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="5"/>
       <c r="E17" s="3"/>
-      <c r="G17" s="15"/>
+      <c r="G17" s="14"/>
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18"/>
-      <c r="C18" s="13"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="5"/>
       <c r="E18" s="3"/>
       <c r="L18" s="6"/>
       <c r="M18" s="4">
-        <f>EXP(C2*G$2+H$2)</f>
+        <f t="shared" ref="M18:M23" si="2">EXP(C2*G$2+H$2)</f>
         <v>0.24335919161903002</v>
       </c>
       <c r="N18"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B19"/>
-      <c r="C19" s="13"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="L19" s="6"/>
       <c r="M19" s="4">
-        <f>EXP(C3*G$2+H$2)</f>
+        <f t="shared" si="2"/>
         <v>0.29882458180953059</v>
       </c>
       <c r="N19"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M20" s="4">
-        <f>EXP(C4*G$2+H$2)</f>
+        <f t="shared" si="2"/>
         <v>0.33932504008839076</v>
       </c>
       <c r="N20"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="G21" s="11"/>
+      <c r="G21" s="10"/>
       <c r="K21" s="6"/>
       <c r="M21" s="4">
-        <f>EXP(C5*G$2+H$2)</f>
+        <f t="shared" si="2"/>
         <v>0.45945787268287569</v>
       </c>
       <c r="N21"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M22" s="4">
-        <f>EXP(C6*G$2+H$2)</f>
+        <f t="shared" si="2"/>
         <v>9.5179535526026662</v>
       </c>
       <c r="N22"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M23" s="4">
-        <f>EXP(C7*G$2+H$2)</f>
+        <f t="shared" si="2"/>
         <v>13.401637245543412</v>
       </c>
       <c r="N23">
@@ -9299,7 +10624,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="3"/>
-      <c r="E34" s="15"/>
+      <c r="E34" s="14"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
@@ -9309,201 +10634,201 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D42" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E42" s="12"/>
+        <v>87</v>
+      </c>
+      <c r="E42" s="11"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D43" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E43" s="12"/>
+        <v>88</v>
+      </c>
+      <c r="E43" s="11"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D44" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E44" s="12"/>
+        <v>89</v>
+      </c>
+      <c r="E44" s="11"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D45" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E45" s="12"/>
+        <v>90</v>
+      </c>
+      <c r="E45" s="11"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D46" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E46" s="12"/>
+        <v>91</v>
+      </c>
+      <c r="E46" s="11"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D47" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E47" s="12"/>
+        <v>92</v>
+      </c>
+      <c r="E47" s="11"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D48" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E48" s="12"/>
+        <v>93</v>
+      </c>
+      <c r="E48" s="11"/>
     </row>
     <row r="49" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D49" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E49" s="12"/>
+        <v>94</v>
+      </c>
+      <c r="E49" s="11"/>
     </row>
     <row r="50" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D50" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E50" s="12"/>
+        <v>95</v>
+      </c>
+      <c r="E50" s="11"/>
     </row>
     <row r="51" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D51" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E51" s="12"/>
+        <v>85</v>
+      </c>
+      <c r="E51" s="11"/>
     </row>
     <row r="52" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D52" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E52" s="12"/>
+        <v>96</v>
+      </c>
+      <c r="E52" s="11"/>
     </row>
     <row r="53" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D53" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E53" s="12"/>
+        <v>86</v>
+      </c>
+      <c r="E53" s="11"/>
     </row>
     <row r="54" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D54" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E54" s="12"/>
+        <v>93</v>
+      </c>
+      <c r="E54" s="11"/>
     </row>
     <row r="55" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D55" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E55" s="12"/>
+        <v>97</v>
+      </c>
+      <c r="E55" s="11"/>
     </row>
     <row r="56" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D56" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E56" s="12"/>
+        <v>98</v>
+      </c>
+      <c r="E56" s="11"/>
     </row>
     <row r="57" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D57" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="E57" s="12"/>
+        <v>99</v>
+      </c>
+      <c r="E57" s="11"/>
     </row>
     <row r="58" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D58" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E58" s="12"/>
+        <v>100</v>
+      </c>
+      <c r="E58" s="11"/>
     </row>
     <row r="59" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D59" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E59" s="12"/>
+        <v>101</v>
+      </c>
+      <c r="E59" s="11"/>
     </row>
     <row r="60" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D60" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E60" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="E60" s="11"/>
     </row>
     <row r="61" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D61" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E61" s="12"/>
+        <v>103</v>
+      </c>
+      <c r="E61" s="11"/>
     </row>
     <row r="62" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D62" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E62" s="12"/>
+        <v>104</v>
+      </c>
+      <c r="E62" s="11"/>
     </row>
     <row r="63" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D63" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E63" s="12"/>
+        <v>105</v>
+      </c>
+      <c r="E63" s="11"/>
     </row>
     <row r="64" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D64" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E64" s="12"/>
+        <v>106</v>
+      </c>
+      <c r="E64" s="11"/>
     </row>
     <row r="65" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D65" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E65" s="12"/>
+        <v>107</v>
+      </c>
+      <c r="E65" s="11"/>
     </row>
     <row r="66" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D66" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E66" s="12"/>
+        <v>108</v>
+      </c>
+      <c r="E66" s="11"/>
     </row>
     <row r="67" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D67" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E67" s="12"/>
+        <v>109</v>
+      </c>
+      <c r="E67" s="11"/>
     </row>
     <row r="68" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D68" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E68" s="12"/>
+        <v>110</v>
+      </c>
+      <c r="E68" s="11"/>
     </row>
     <row r="69" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D69" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E69" s="12"/>
+        <v>93</v>
+      </c>
+      <c r="E69" s="11"/>
     </row>
     <row r="70" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D70" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E70" s="12"/>
+        <v>111</v>
+      </c>
+      <c r="E70" s="11"/>
     </row>
     <row r="71" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D71" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E71" s="12"/>
+        <v>112</v>
+      </c>
+      <c r="E71" s="11"/>
     </row>
     <row r="72" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D72" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E72" s="12"/>
+        <v>113</v>
+      </c>
+      <c r="E72" s="11"/>
     </row>
     <row r="73" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D73" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E73" s="12"/>
+        <v>85</v>
+      </c>
+      <c r="E73" s="11"/>
     </row>
     <row r="74" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D74" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E74" s="12"/>
+        <v>103</v>
+      </c>
+      <c r="E74" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>